<commit_message>
Updated Transport Usage by Income + Clustering as well as reordering the data file
</commit_message>
<xml_diff>
--- a/data/transportmodevsIncome.xlsx
+++ b/data/transportmodevsIncome.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/45bfc195ac2ed6ff/Documents/GitHub/Analyzing-NSW-Public-Transports-with-Opal-Cards/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{64882914-0AF5-4E72-B669-D4D5D2D29720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF372D3F-057D-4B21-8EFA-A51239120520}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{64882914-0AF5-4E72-B669-D4D5D2D29720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F32E6FB-695C-4761-9EAD-1272FA45694A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>New South Wales</t>
   </si>
   <si>
-    <t>INCP Total Personal Income (weekly)</t>
-  </si>
-  <si>
     <t>Nil income</t>
   </si>
   <si>
@@ -168,6 +165,9 @@
   </si>
   <si>
     <t>$3,000 or more($156,000 or more)</t>
+  </si>
+  <si>
+    <t>INCP Total Personal Income: weekly (annually)</t>
   </si>
 </sst>
 </file>
@@ -432,6 +432,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -632,9 +636,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P7" sqref="P7"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -698,6 +702,7 @@
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -706,76 +711,77 @@
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="H10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="I10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="J10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="K10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="L10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="N10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="N10" s="11" t="s">
+      <c r="O10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="O10" s="11" t="s">
+      <c r="P10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="P10" s="11" t="s">
+      <c r="Q10" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="R10" s="11" t="s">
         <v>22</v>
-      </c>
-      <c r="Q10" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="R10" s="11" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="3">
+        <v>350</v>
+      </c>
+      <c r="D12" s="3">
         <v>1070</v>
-      </c>
-      <c r="D12" s="3">
-        <v>350</v>
       </c>
       <c r="E12" s="3">
         <v>6028</v>
@@ -822,13 +828,13 @@
     </row>
     <row r="13" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="3">
+        <v>25</v>
+      </c>
+      <c r="C13" s="7">
+        <v>147</v>
+      </c>
+      <c r="D13" s="3">
         <v>547</v>
-      </c>
-      <c r="D13" s="7">
-        <v>147</v>
       </c>
       <c r="E13" s="3">
         <v>5454</v>
@@ -875,13 +881,13 @@
     </row>
     <row r="14" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="3">
+        <v>22</v>
+      </c>
+      <c r="D14" s="7">
         <v>27</v>
-      </c>
-      <c r="C14" s="7">
-        <v>27</v>
-      </c>
-      <c r="D14" s="3">
-        <v>22</v>
       </c>
       <c r="E14" s="3">
         <v>53</v>
@@ -928,13 +934,13 @@
     </row>
     <row r="15" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="3">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3">
         <v>7</v>
-      </c>
-      <c r="D15" s="3">
-        <v>10</v>
       </c>
       <c r="E15" s="3">
         <v>54</v>
@@ -981,13 +987,13 @@
     </row>
     <row r="16" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="3">
+        <v>530</v>
+      </c>
+      <c r="D16" s="3">
         <v>1650</v>
-      </c>
-      <c r="D16" s="3">
-        <v>530</v>
       </c>
       <c r="E16" s="3">
         <v>11586</v>
@@ -1032,41 +1038,42 @@
         <v>533614</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="B19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="3"/>
     </row>
-    <row r="18" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="3" t="s">
+    <row r="20" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+    <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2089,17 +2096,17 @@
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2107,12 +2114,12 @@
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3129,37 +3136,37 @@
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="10">
         <v>0.25</v>
@@ -3167,10 +3174,10 @@
     </row>
     <row r="8" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>